<commit_message>
05-08-2023 Advance JS completed Simon Game start DA recap needed and Subcategorisation proceeded
</commit_message>
<xml_diff>
--- a/Data-Science/Projects/Live-Project/Categorisation.xlsx
+++ b/Data-Science/Projects/Live-Project/Categorisation.xlsx
@@ -24,7 +24,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Sub-Category</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>First Seen</t>
+  </si>
+  <si>
+    <t>Last Seen</t>
+  </si>
+  <si>
+    <t>04_Salary</t>
+  </si>
+  <si>
+    <t>Pankaj</t>
+  </si>
+  <si>
+    <t>02_Gas</t>
+  </si>
+  <si>
+    <t>HP gas(all big+small)</t>
+  </si>
+  <si>
+    <t>01_Kirana</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>Wheel Powder</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -66,12 +106,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -354,23 +397,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="17.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="2"/>
+    <col min="5" max="6" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2">
+        <v>28300</v>
+      </c>
+      <c r="E2" s="3">
+        <v>45011</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>81</v>
+      </c>
+      <c r="D3" s="2">
+        <v>135290</v>
+      </c>
+      <c r="E3" s="3">
+        <v>44927</v>
+      </c>
+      <c r="F3" s="3">
+        <v>45086</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3070</v>
+      </c>
+      <c r="E4" s="3">
+        <v>44978</v>
+      </c>
+      <c r="F4" s="3">
+        <v>45106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>222</v>
+      </c>
+      <c r="E5" s="3">
+        <v>44930</v>
+      </c>
+      <c r="F5" s="3">
+        <v>45064</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
07-08-2023 Completed with with some categorization
</commit_message>
<xml_diff>
--- a/Data-Science/Projects/Live-Project/Categorisation.xlsx
+++ b/Data-Science/Projects/Live-Project/Categorisation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Category</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Wheel Powder</t>
+  </si>
+  <si>
+    <t>Sugar</t>
+  </si>
+  <si>
+    <t>Vinegar</t>
   </si>
 </sst>
 </file>
@@ -397,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,6 +520,46 @@
         <v>45064</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>125</v>
+      </c>
+      <c r="E6" s="3">
+        <v>44936</v>
+      </c>
+      <c r="F6" s="3">
+        <v>45008</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3">
+        <v>44946</v>
+      </c>
+      <c r="F7" s="3">
+        <v>44946</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>